<commit_message>
updated version Nov 26 2024
</commit_message>
<xml_diff>
--- a/scripts/templates/wholeCNS_region_definitions_cordsegments.xlsx
+++ b/scripts/templates/wholeCNS_region_definitions_cordsegments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16135\PycharmProjects\pantheon\venv\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stroman\PycharmProjects\pantheon\scripts\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE52EC8-E094-4F98-8133-0CE119815704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD558184-F304-4483-A827-3586F855CBCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="760" windowWidth="17890" windowHeight="9250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11980" yWindow="2430" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="435">
   <si>
     <t>number</t>
   </si>
@@ -1687,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E251"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D130" sqref="D130"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5964,6 +5964,20 @@
         <v>96</v>
       </c>
     </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A252">
+        <v>250</v>
+      </c>
+      <c r="B252">
+        <v>251</v>
+      </c>
+      <c r="C252" t="s">
+        <v>185</v>
+      </c>
+      <c r="D252" t="s">
+        <v>185</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>